<commit_message>
Overdue data is included.
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-ChangeNote.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-ChangeNote.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Transmittals_New_ActionRequired" sheetId="1" r:id="rId1"/>
+    <sheet name="Transmittals_New_ActionOverDue" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>To</t>
   </si>
@@ -107,6 +108,12 @@
   </si>
   <si>
     <t>Approved</t>
+  </si>
+  <si>
+    <t>Overdue</t>
+  </si>
+  <si>
+    <t>LATFULPP-4</t>
   </si>
 </sst>
 </file>
@@ -187,13 +194,7 @@
       <sheetName val="DocumentDetails"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>AutoTestAdmin</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="B2" t="str">
@@ -563,7 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -692,4 +693,139 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" t="str">
+        <f>[1]DocumentDetails!$B$2</f>
+        <v>Document Register</v>
+      </c>
+      <c r="K2" t="str">
+        <f>[2]DocumentDetails!$B$3</f>
+        <v>ATCRL-AOT-ACV-BIM-002436.docx</v>
+      </c>
+      <c r="L2" t="str">
+        <f>[1]DocumentDetails!$B$2</f>
+        <v>Document Register</v>
+      </c>
+      <c r="M2" t="str">
+        <f>[2]DocumentDetails!$B$4</f>
+        <v>ATCRL-AOT-ACV-BIM-002436.docx</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>